<commit_message>
Add web scrapping to two distribuitors and fix bugs in the code
</commit_message>
<xml_diff>
--- a/homologación/nuevos.xlsx
+++ b/homologación/nuevos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpiscoya\OneDrive - Laive\Documentos\python-projects\homologación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C107789-72A1-49DA-AC97-F222AEE3CA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558A63C2-EADA-49C2-809F-9CF937A9ECEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{62428D55-77F9-4330-ADC7-D593BE507B78}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>SAP</t>
   </si>
@@ -47,39 +47,6 @@
     <t>PESO</t>
   </si>
   <si>
-    <t>PROM. HOT DOG SUIZA PQT 200G</t>
-  </si>
-  <si>
-    <t>15+1</t>
-  </si>
-  <si>
-    <t>PROM. JAMONADA CON POLLO SUIZA PQT 100G</t>
-  </si>
-  <si>
-    <t>PROM. JAMONADA ESPECIAL SUIZA PQT 100G</t>
-  </si>
-  <si>
-    <t>PROM. JAMONADA ESPECIAL SUIZA MOLDE 2KG</t>
-  </si>
-  <si>
-    <t>PROM. CHICHARRON DE PRENSA SUIZA MOLDE</t>
-  </si>
-  <si>
-    <t>PROM. JAMON AMERICANO SUIZA MOLDE</t>
-  </si>
-  <si>
-    <t>PROM. JAMONADA CON POLLO SUIZA MOLDE 2KG</t>
-  </si>
-  <si>
-    <t>PROM. QUESO MOZZARELLA PIZZERO MOLDE</t>
-  </si>
-  <si>
-    <t>PROM. QUESO EDAM TAJADAS FINAS PQT 90G</t>
-  </si>
-  <si>
-    <t>PROM. QUESO EDAM LAIVE MOLDE</t>
-  </si>
-  <si>
     <t>UNIFLEX</t>
   </si>
   <si>
@@ -87,6 +54,78 @@
   </si>
   <si>
     <t>ESPROMO</t>
+  </si>
+  <si>
+    <t>0225</t>
+  </si>
+  <si>
+    <t>50000077</t>
+  </si>
+  <si>
+    <t>Q. LAIVE EDAM SANDWICH (S/I) PQT 500G</t>
+  </si>
+  <si>
+    <t>TOCINO AHUM. SUIZA TAJADAS BOLSA</t>
+  </si>
+  <si>
+    <t>50000217</t>
+  </si>
+  <si>
+    <t>3646</t>
+  </si>
+  <si>
+    <t>50000353</t>
+  </si>
+  <si>
+    <t>Q. CREMA BAZO VELARDE POTE 1KG</t>
+  </si>
+  <si>
+    <t>0344</t>
+  </si>
+  <si>
+    <t>50000401</t>
+  </si>
+  <si>
+    <t>FRANKFURTER XL SUIZA PAQUETE 1KG</t>
+  </si>
+  <si>
+    <t>3623</t>
+  </si>
+  <si>
+    <t>50000441</t>
+  </si>
+  <si>
+    <t>QUESO PARMESANO LAIVE CHEF</t>
+  </si>
+  <si>
+    <t>0281</t>
+  </si>
+  <si>
+    <t>50000599</t>
+  </si>
+  <si>
+    <t>DULCE DE LECHE BAZO VELARDE X 13.6 Kg</t>
+  </si>
+  <si>
+    <t>9070</t>
+  </si>
+  <si>
+    <t>50000616</t>
+  </si>
+  <si>
+    <t>QUESO EDAM LAIVE CHEF MOLDE</t>
+  </si>
+  <si>
+    <t>0226</t>
+  </si>
+  <si>
+    <t>50000831</t>
+  </si>
+  <si>
+    <t>DULCE DE LECHE BAZO VELARDE 5KG</t>
+  </si>
+  <si>
+    <t>9071</t>
   </si>
 </sst>
 </file>
@@ -190,11 +229,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -221,6 +257,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -560,327 +602,285 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="46" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="8"/>
+    <col min="1" max="1" width="13.109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="46" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>9053</v>
-      </c>
-      <c r="B2" s="5">
-        <v>50000913</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="F2" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>9054</v>
-      </c>
-      <c r="B3" s="5">
-        <v>50000251</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6">
+        <v>9.1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
+        <v>13.6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
+        <v>3.21</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>9055</v>
-      </c>
-      <c r="B4" s="5">
-        <v>50000250</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>9056</v>
-      </c>
-      <c r="B5" s="5">
-        <v>50000714</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>9057</v>
-      </c>
-      <c r="B6" s="5">
-        <v>50000249</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>9058</v>
-      </c>
-      <c r="B7" s="5">
-        <v>50000203</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2.6</v>
-      </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>9059</v>
-      </c>
-      <c r="B8" s="5">
-        <v>50000712</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>9060</v>
-      </c>
-      <c r="B9" s="5">
-        <v>80000177</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2.7</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
+      <c r="F9" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>9061</v>
-      </c>
-      <c r="B10" s="5">
-        <v>50000073</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="F10" s="7">
-        <v>1</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>9062</v>
-      </c>
-      <c r="B11" s="5">
-        <v>50000292</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>